<commit_message>
add dancing links solution v1.1
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -49,7 +49,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -69,6 +69,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC166"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -244,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="50">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -252,58 +258,58 @@
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="0" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="0" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="9" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="10" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="9" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="10" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -312,102 +318,6 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="3" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf applyAlignment="1" borderId="2" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -417,88 +327,76 @@
     <xf applyAlignment="1" borderId="4" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="5" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="9" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="10" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="6" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="6" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="6" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="7" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="7" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="6" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="6" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="7" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="5" fillId="6" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="8" fillId="6" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="9" fillId="7" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="10" fillId="6" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="9" fillId="6" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="10" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="6" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="5" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="6" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="6" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="6" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="7" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="7" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="7" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="7" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="10" fillId="7" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -801,190 +699,194 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R8" sqref="A1:XFD1048576"/>
+      <selection activeCell="P9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" style="21" width="8.25"/>
-    <col bestFit="1" customWidth="1" max="5" min="2" style="22" width="8.25"/>
-    <col bestFit="1" customWidth="1" max="11" min="6" style="21" width="8.25"/>
+    <col bestFit="1" customWidth="1" max="10" min="2" style="22" width="8.25"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="21" width="8.25"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="50.1" r="1" spans="1:11">
+    <row customHeight="1" ht="18.75" r="1" spans="1:11" thickBot="1">
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="n"/>
       <c r="C1" s="2" t="n"/>
       <c r="D1" s="2" t="n"/>
       <c r="E1" s="2" t="n"/>
-      <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
-      <c r="I1" s="1" t="n"/>
-      <c r="J1" s="1" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
       <c r="K1" s="1" t="n"/>
     </row>
-    <row customHeight="1" ht="50.1" r="2" spans="1:11">
+    <row customHeight="1" ht="47.25" r="2" spans="1:11">
       <c r="A2" s="1" t="n"/>
-      <c r="B2" s="5" t="n"/>
-      <c r="C2" s="3" t="n"/>
-      <c r="D2" s="4" t="n"/>
-      <c r="E2" s="5" t="n"/>
-      <c r="F2" s="6" t="n">
+      <c r="B2" s="23" t="n"/>
+      <c r="C2" s="24" t="n"/>
+      <c r="D2" s="25" t="n"/>
+      <c r="E2" s="23" t="n"/>
+      <c r="F2" s="24" t="n">
         <v>6</v>
       </c>
-      <c r="G2" s="7" t="n"/>
-      <c r="H2" s="8" t="n"/>
-      <c r="I2" s="6" t="n"/>
-      <c r="J2" s="7" t="n"/>
+      <c r="G2" s="25" t="n"/>
+      <c r="H2" s="23" t="n"/>
+      <c r="I2" s="24" t="n"/>
+      <c r="J2" s="25" t="n"/>
       <c r="K2" s="1" t="n"/>
     </row>
-    <row customHeight="1" ht="50.1" r="3" spans="1:11">
+    <row customHeight="1" ht="47.25" r="3" spans="1:11">
       <c r="A3" s="1" t="n"/>
-      <c r="B3" s="9" t="n">
+      <c r="B3" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="C3" s="19" t="n"/>
-      <c r="D3" s="10" t="n"/>
-      <c r="E3" s="9" t="n">
+      <c r="C3" s="27" t="n"/>
+      <c r="D3" s="28" t="n"/>
+      <c r="E3" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="11" t="n"/>
-      <c r="G3" s="12" t="n">
+      <c r="F3" s="27" t="n"/>
+      <c r="G3" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="H3" s="13" t="n"/>
-      <c r="I3" s="11" t="n"/>
-      <c r="J3" s="12" t="n">
+      <c r="H3" s="26" t="n"/>
+      <c r="I3" s="27" t="n"/>
+      <c r="J3" s="28" t="n">
         <v>9</v>
       </c>
       <c r="K3" s="1" t="n"/>
     </row>
-    <row customHeight="1" ht="50.1" r="4" spans="1:11">
+    <row customHeight="1" ht="48" r="4" spans="1:11" thickBot="1">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="14" t="n"/>
-      <c r="C4" s="15" t="n">
+      <c r="B4" s="29" t="n"/>
+      <c r="C4" s="30" t="n">
         <v>6</v>
       </c>
-      <c r="D4" s="20" t="n"/>
-      <c r="E4" s="14" t="n"/>
-      <c r="F4" s="16" t="n"/>
-      <c r="G4" s="17" t="n"/>
-      <c r="H4" s="18" t="n"/>
-      <c r="I4" s="16" t="n">
+      <c r="D4" s="31" t="n"/>
+      <c r="E4" s="29" t="n"/>
+      <c r="F4" s="30" t="n"/>
+      <c r="G4" s="31" t="n"/>
+      <c r="H4" s="29" t="n"/>
+      <c r="I4" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="J4" s="17" t="n"/>
+      <c r="J4" s="31" t="n"/>
       <c r="K4" s="1" t="n"/>
     </row>
-    <row customHeight="1" ht="50.1" r="5" spans="1:11">
+    <row customHeight="1" ht="47.25" r="5" spans="1:11">
       <c r="A5" s="1" t="n"/>
-      <c r="B5" s="5" t="n"/>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="4" t="n"/>
-      <c r="E5" s="5" t="n">
+      <c r="B5" s="23" t="n"/>
+      <c r="C5" s="24" t="n"/>
+      <c r="D5" s="25" t="n"/>
+      <c r="E5" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="F5" s="6" t="n"/>
-      <c r="G5" s="7" t="n">
+      <c r="F5" s="24" t="n"/>
+      <c r="G5" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="H5" s="8" t="n"/>
-      <c r="I5" s="6" t="n"/>
-      <c r="J5" s="7" t="n"/>
+      <c r="H5" s="23" t="n"/>
+      <c r="I5" s="24" t="n"/>
+      <c r="J5" s="25" t="n"/>
       <c r="K5" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="50.1" r="6" spans="1:11">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="9" t="n"/>
-      <c r="C6" s="19" t="n"/>
-      <c r="D6" s="10" t="n">
+      <c r="B6" s="26" t="n"/>
+      <c r="C6" s="27" t="n"/>
+      <c r="D6" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="9" t="n"/>
-      <c r="F6" s="23" t="n">
+      <c r="E6" s="26" t="n"/>
+      <c r="F6" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="12" t="n"/>
-      <c r="H6" s="13" t="n">
+      <c r="G6" s="28" t="n"/>
+      <c r="H6" s="26" t="n">
         <v>9</v>
       </c>
-      <c r="I6" s="11" t="n"/>
-      <c r="J6" s="12" t="n"/>
+      <c r="I6" s="27" t="n"/>
+      <c r="J6" s="28" t="n"/>
       <c r="K6" s="1" t="n"/>
     </row>
-    <row customHeight="1" ht="50.1" r="7" spans="1:11">
+    <row customHeight="1" ht="50.1" r="7" spans="1:11" thickBot="1">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="14" t="n"/>
-      <c r="C7" s="15" t="n">
+      <c r="B7" s="29" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" s="30" t="n">
         <v>8</v>
       </c>
-      <c r="D7" s="20" t="n"/>
-      <c r="E7" s="14" t="n"/>
-      <c r="F7" s="16" t="n"/>
-      <c r="G7" s="17" t="n"/>
-      <c r="H7" s="18" t="n"/>
-      <c r="I7" s="16" t="n">
+      <c r="D7" s="31" t="n"/>
+      <c r="E7" s="29" t="n"/>
+      <c r="F7" s="30" t="n"/>
+      <c r="G7" s="31" t="n"/>
+      <c r="H7" s="29" t="n"/>
+      <c r="I7" s="30" t="n">
         <v>7</v>
       </c>
-      <c r="J7" s="17" t="n"/>
+      <c r="J7" s="31" t="n"/>
       <c r="K7" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="50.1" r="8" spans="1:11">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="5" t="n"/>
-      <c r="C8" s="3" t="n"/>
-      <c r="D8" s="4" t="n">
+      <c r="B8" s="23" t="n"/>
+      <c r="C8" s="24" t="n"/>
+      <c r="D8" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="E8" s="5" t="n"/>
-      <c r="F8" s="6" t="n"/>
-      <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="n">
+      <c r="E8" s="23" t="n"/>
+      <c r="F8" s="24" t="n"/>
+      <c r="G8" s="25" t="n"/>
+      <c r="H8" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="I8" s="6" t="n"/>
-      <c r="J8" s="7" t="n"/>
+      <c r="I8" s="24" t="n"/>
+      <c r="J8" s="25" t="n"/>
       <c r="K8" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="50.1" r="9" spans="1:11">
       <c r="A9" s="1" t="n"/>
-      <c r="B9" s="9" t="n">
+      <c r="B9" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="19" t="n"/>
-      <c r="D9" s="10" t="n"/>
-      <c r="E9" s="9" t="n"/>
-      <c r="F9" s="11" t="n">
+      <c r="C9" s="27" t="n"/>
+      <c r="D9" s="28" t="n"/>
+      <c r="E9" s="26" t="n"/>
+      <c r="F9" s="27" t="n">
         <v>8</v>
       </c>
-      <c r="G9" s="12" t="n"/>
-      <c r="H9" s="13" t="n"/>
-      <c r="I9" s="11" t="n"/>
-      <c r="J9" s="12" t="n">
+      <c r="G9" s="28" t="n"/>
+      <c r="H9" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="27" t="n"/>
+      <c r="J9" s="28" t="n">
         <v>4</v>
       </c>
       <c r="K9" s="1" t="n"/>
     </row>
-    <row customHeight="1" ht="50.1" r="10" spans="1:11">
+    <row customHeight="1" ht="50.1" r="10" spans="1:11" thickBot="1">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="14" t="n"/>
-      <c r="C10" s="15" t="n">
+      <c r="B10" s="29" t="n"/>
+      <c r="C10" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="D10" s="20" t="n"/>
-      <c r="E10" s="14" t="n">
+      <c r="D10" s="31" t="n"/>
+      <c r="E10" s="29" t="n">
         <v>4</v>
       </c>
-      <c r="F10" s="16" t="n"/>
-      <c r="G10" s="17" t="n">
+      <c r="F10" s="30" t="n"/>
+      <c r="G10" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="H10" s="18" t="n"/>
-      <c r="I10" s="16" t="n">
+      <c r="H10" s="29" t="n"/>
+      <c r="I10" s="30" t="n">
         <v>6</v>
       </c>
-      <c r="J10" s="17" t="n"/>
+      <c r="J10" s="31" t="n"/>
       <c r="K10" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="50.1" r="11" spans="1:11">
@@ -993,11 +895,11 @@
       <c r="C11" s="2" t="n"/>
       <c r="D11" s="2" t="n"/>
       <c r="E11" s="2" t="n"/>
-      <c r="F11" s="1" t="n"/>
-      <c r="G11" s="1" t="n"/>
-      <c r="H11" s="1" t="n"/>
-      <c r="I11" s="1" t="n"/>
-      <c r="J11" s="1" t="n"/>
+      <c r="F11" s="2" t="n"/>
+      <c r="G11" s="2" t="n"/>
+      <c r="H11" s="2" t="n"/>
+      <c r="I11" s="2" t="n"/>
+      <c r="J11" s="2" t="n"/>
       <c r="K11" s="1" t="n"/>
     </row>
   </sheetData>
@@ -1015,14 +917,14 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="A1:XFD1048576"/>
+      <selection activeCell="Q7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" style="21" width="8.25"/>
-    <col bestFit="1" customWidth="1" max="5" min="2" style="22" width="8.25"/>
-    <col bestFit="1" customWidth="1" max="11" min="6" style="21" width="8.25"/>
+    <col bestFit="1" customWidth="1" max="10" min="2" style="22" width="8.25"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="21" width="8.25"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="19.5" r="1" spans="1:11">
@@ -1031,288 +933,288 @@
       <c r="C1" s="2" t="n"/>
       <c r="D1" s="2" t="n"/>
       <c r="E1" s="2" t="n"/>
-      <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
-      <c r="I1" s="1" t="n"/>
-      <c r="J1" s="1" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
       <c r="K1" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="47.25" r="2" spans="1:11">
       <c r="A2" s="1" t="n"/>
-      <c r="B2" s="55" t="n">
+      <c r="B2" s="32" t="n">
         <v>4</v>
       </c>
-      <c r="C2" s="56" t="n">
+      <c r="C2" s="33" t="n">
         <v>9</v>
       </c>
-      <c r="D2" s="57" t="n">
+      <c r="D2" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="E2" s="55" t="n">
+      <c r="E2" s="32" t="n">
         <v>8</v>
       </c>
-      <c r="F2" s="58" t="n">
+      <c r="F2" s="35" t="n">
         <v>6</v>
       </c>
-      <c r="G2" s="59" t="n">
+      <c r="G2" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="H2" s="60" t="n">
+      <c r="H2" s="32" t="n">
         <v>7</v>
       </c>
-      <c r="I2" s="61" t="n">
+      <c r="I2" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="59" t="n">
+      <c r="J2" s="34" t="n">
         <v>5</v>
       </c>
       <c r="K2" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="47.25" r="3" spans="1:11">
       <c r="A3" s="1" t="n"/>
-      <c r="B3" s="62" t="n">
+      <c r="B3" s="36" t="n">
         <v>3</v>
       </c>
-      <c r="C3" s="63" t="n">
+      <c r="C3" s="37" t="n">
         <v>7</v>
       </c>
-      <c r="D3" s="64" t="n">
+      <c r="D3" s="38" t="n">
         <v>8</v>
       </c>
-      <c r="E3" s="62" t="n">
+      <c r="E3" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="65" t="n">
+      <c r="F3" s="37" t="n">
         <v>4</v>
       </c>
-      <c r="G3" s="66" t="n">
+      <c r="G3" s="39" t="n">
         <v>5</v>
       </c>
-      <c r="H3" s="67" t="n">
+      <c r="H3" s="40" t="n">
         <v>6</v>
       </c>
-      <c r="I3" s="65" t="n">
+      <c r="I3" s="37" t="n">
         <v>2</v>
       </c>
-      <c r="J3" s="66" t="n">
+      <c r="J3" s="39" t="n">
         <v>9</v>
       </c>
       <c r="K3" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="48" r="4" spans="1:11">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="68" t="n">
+      <c r="B4" s="41" t="n">
         <v>5</v>
       </c>
-      <c r="C4" s="69" t="n">
+      <c r="C4" s="42" t="n">
         <v>6</v>
       </c>
-      <c r="D4" s="70" t="n">
+      <c r="D4" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="68" t="n">
+      <c r="E4" s="41" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="71" t="n">
+      <c r="F4" s="44" t="n">
         <v>7</v>
       </c>
-      <c r="G4" s="72" t="n">
+      <c r="G4" s="43" t="n">
         <v>9</v>
       </c>
-      <c r="H4" s="73" t="n">
+      <c r="H4" s="41" t="n">
         <v>8</v>
       </c>
-      <c r="I4" s="74" t="n">
+      <c r="I4" s="42" t="n">
         <v>4</v>
       </c>
-      <c r="J4" s="72" t="n">
+      <c r="J4" s="43" t="n">
         <v>3</v>
       </c>
       <c r="K4" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="47.25" r="5" spans="1:11">
       <c r="A5" s="1" t="n"/>
-      <c r="B5" s="55" t="n">
+      <c r="B5" s="32" t="n">
         <v>7</v>
       </c>
-      <c r="C5" s="56" t="n">
+      <c r="C5" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="57" t="n">
+      <c r="D5" s="34" t="n">
         <v>5</v>
       </c>
-      <c r="E5" s="75" t="n">
+      <c r="E5" s="45" t="n">
         <v>6</v>
       </c>
-      <c r="F5" s="61" t="n">
+      <c r="F5" s="33" t="n">
         <v>9</v>
       </c>
-      <c r="G5" s="76" t="n">
+      <c r="G5" s="46" t="n">
         <v>2</v>
       </c>
-      <c r="H5" s="60" t="n">
+      <c r="H5" s="32" t="n">
         <v>4</v>
       </c>
-      <c r="I5" s="61" t="n">
+      <c r="I5" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="J5" s="59" t="n">
+      <c r="J5" s="34" t="n">
         <v>8</v>
       </c>
       <c r="K5" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="47.25" r="6" spans="1:11">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="77" t="n">
+      <c r="B6" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="63" t="n">
+      <c r="C6" s="37" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="78" t="n">
+      <c r="D6" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="77" t="n">
+      <c r="E6" s="40" t="n">
         <v>7</v>
       </c>
-      <c r="F6" s="79" t="n">
+      <c r="F6" s="47" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="80" t="n">
+      <c r="G6" s="38" t="n">
         <v>8</v>
       </c>
-      <c r="H6" s="81" t="n">
+      <c r="H6" s="36" t="n">
         <v>9</v>
       </c>
-      <c r="I6" s="65" t="n">
+      <c r="I6" s="37" t="n">
         <v>5</v>
       </c>
-      <c r="J6" s="80" t="n">
+      <c r="J6" s="38" t="n">
         <v>6</v>
       </c>
       <c r="K6" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="48" r="7" spans="1:11">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="68" t="n">
+      <c r="B7" s="48" t="n">
         <v>9</v>
       </c>
-      <c r="C7" s="69" t="n">
+      <c r="C7" s="42" t="n">
         <v>8</v>
       </c>
-      <c r="D7" s="70" t="n">
+      <c r="D7" s="43" t="n">
         <v>6</v>
       </c>
-      <c r="E7" s="68" t="n">
+      <c r="E7" s="41" t="n">
         <v>3</v>
       </c>
-      <c r="F7" s="71" t="n">
+      <c r="F7" s="44" t="n">
         <v>5</v>
       </c>
-      <c r="G7" s="72" t="n">
+      <c r="G7" s="43" t="n">
         <v>4</v>
       </c>
-      <c r="H7" s="73" t="n">
+      <c r="H7" s="41" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="74" t="n">
+      <c r="I7" s="42" t="n">
         <v>7</v>
       </c>
-      <c r="J7" s="72" t="n">
+      <c r="J7" s="43" t="n">
         <v>2</v>
       </c>
       <c r="K7" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="47.25" r="8" spans="1:11">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="55" t="n">
+      <c r="B8" s="32" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="56" t="n">
+      <c r="C8" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="82" t="n">
+      <c r="D8" s="46" t="n">
         <v>4</v>
       </c>
-      <c r="E8" s="55" t="n">
+      <c r="E8" s="32" t="n">
         <v>9</v>
       </c>
-      <c r="F8" s="61" t="n">
+      <c r="F8" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="59" t="n">
+      <c r="G8" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="83" t="n">
+      <c r="H8" s="45" t="n">
         <v>3</v>
       </c>
-      <c r="I8" s="61" t="n">
+      <c r="I8" s="33" t="n">
         <v>8</v>
       </c>
-      <c r="J8" s="59" t="n">
+      <c r="J8" s="34" t="n">
         <v>7</v>
       </c>
       <c r="K8" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="50.1" r="9" spans="1:11">
       <c r="A9" s="1" t="n"/>
-      <c r="B9" s="62" t="n">
+      <c r="B9" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="63" t="n">
+      <c r="C9" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="D9" s="64" t="n">
+      <c r="D9" s="38" t="n">
         <v>7</v>
       </c>
-      <c r="E9" s="77" t="n">
+      <c r="E9" s="40" t="n">
         <v>5</v>
       </c>
-      <c r="F9" s="79" t="n">
+      <c r="F9" s="47" t="n">
         <v>8</v>
       </c>
-      <c r="G9" s="80" t="n">
+      <c r="G9" s="38" t="n">
         <v>6</v>
       </c>
-      <c r="H9" s="67" t="n">
+      <c r="H9" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="65" t="n">
+      <c r="I9" s="37" t="n">
         <v>9</v>
       </c>
-      <c r="J9" s="66" t="n">
+      <c r="J9" s="39" t="n">
         <v>4</v>
       </c>
       <c r="K9" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="50.1" r="10" spans="1:11">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="68" t="n">
+      <c r="B10" s="41" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="69" t="n">
+      <c r="C10" s="42" t="n">
         <v>2</v>
       </c>
-      <c r="D10" s="70" t="n">
+      <c r="D10" s="43" t="n">
         <v>9</v>
       </c>
-      <c r="E10" s="84" t="n">
+      <c r="E10" s="48" t="n">
         <v>4</v>
       </c>
-      <c r="F10" s="71" t="n">
+      <c r="F10" s="44" t="n">
         <v>3</v>
       </c>
-      <c r="G10" s="85" t="n">
+      <c r="G10" s="49" t="n">
         <v>7</v>
       </c>
-      <c r="H10" s="73" t="n">
+      <c r="H10" s="41" t="n">
         <v>5</v>
       </c>
-      <c r="I10" s="74" t="n">
+      <c r="I10" s="42" t="n">
         <v>6</v>
       </c>
-      <c r="J10" s="72" t="n">
+      <c r="J10" s="43" t="n">
         <v>1</v>
       </c>
       <c r="K10" s="1" t="n"/>
@@ -1323,11 +1225,11 @@
       <c r="C11" s="2" t="n"/>
       <c r="D11" s="2" t="n"/>
       <c r="E11" s="2" t="n"/>
-      <c r="F11" s="1" t="n"/>
-      <c r="G11" s="1" t="n"/>
-      <c r="H11" s="1" t="n"/>
-      <c r="I11" s="1" t="n"/>
-      <c r="J11" s="1" t="n"/>
+      <c r="F11" s="2" t="n"/>
+      <c r="G11" s="2" t="n"/>
+      <c r="H11" s="2" t="n"/>
+      <c r="I11" s="2" t="n"/>
+      <c r="J11" s="2" t="n"/>
       <c r="K11" s="1" t="n"/>
     </row>
   </sheetData>

</xml_diff>